<commit_message>
WBS uppdaterad med tidsåtgång för arbetspaket
</commit_message>
<xml_diff>
--- a/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
+++ b/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beije\Documents\Projektkurs DVA227\Bolaget\Förstudie\WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9FD8387-0B4E-4E8B-A2BD-0FAE232E88B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C383E-67EB-46B2-80C7-314518F8D840}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{27FDFA86-4B27-4D7C-8CA5-C51076384BD6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Ta fram en checklista för tester som ska utföras för att siten ska vara godkänd</t>
   </si>
   <si>
-    <t>Definiera listan på saker som ska kollas</t>
-  </si>
-  <si>
     <t>Planera och genomföra mässan I slutet av kursen</t>
   </si>
   <si>
@@ -319,6 +316,21 @@
   </si>
   <si>
     <t>Tidsåtgång</t>
+  </si>
+  <si>
+    <t>Switching</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>Undersöka vad för typ av switchar som passar klienten, baserat på minimikraven</t>
+  </si>
+  <si>
+    <t>Definiera listan på saker som ska kollas, och generellt hur</t>
+  </si>
+  <si>
+    <t>Total tid (Tidsåtgång x resurs)</t>
   </si>
 </sst>
 </file>
@@ -673,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37737CB-10EF-4991-AA29-BCEE5EE5F7F0}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +700,7 @@
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,13 +711,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -713,10 +728,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -727,7 +742,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -737,357 +752,630 @@
       <c r="C4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>1.2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>1.3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>1.4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0.5</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
+      <c r="F28">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>92</v>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <f>SUM(E4:E37)</f>
+        <v>84</v>
+      </c>
+      <c r="F38">
+        <f>SUM(F4:F37)</f>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uppdatering av WBS samt CSV
</commit_message>
<xml_diff>
--- a/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
+++ b/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">Färdigställ rapport och skicka in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt:</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -500,7 +503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -517,10 +520,11 @@
         <v>8</v>
       </c>
       <c r="F4" s="0" t="n">
+        <f aca="false">D4*E4</f>
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -537,10 +541,11 @@
         <v>8</v>
       </c>
       <c r="F5" s="0" t="n">
+        <f aca="false">D5*E5</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -557,10 +562,11 @@
         <v>4</v>
       </c>
       <c r="F6" s="0" t="n">
+        <f aca="false">D6*E6</f>
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -577,10 +583,11 @@
         <v>4</v>
       </c>
       <c r="F7" s="0" t="n">
+        <f aca="false">D7*E7</f>
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -597,10 +604,11 @@
         <v>8</v>
       </c>
       <c r="F8" s="0" t="n">
+        <f aca="false">D8*E8</f>
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -617,10 +625,11 @@
         <v>4</v>
       </c>
       <c r="F9" s="0" t="n">
+        <f aca="false">D9*E9</f>
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -631,7 +640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -648,10 +657,11 @@
         <v>5</v>
       </c>
       <c r="F11" s="0" t="n">
+        <f aca="false">D11*E11</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -668,10 +678,11 @@
         <v>4</v>
       </c>
       <c r="F12" s="0" t="n">
+        <f aca="false">D12*E12</f>
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -688,10 +699,11 @@
         <v>2</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D13*E13</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -708,10 +720,11 @@
         <v>2</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D14*E14</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -728,10 +741,11 @@
         <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D15*E15</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -748,10 +762,11 @@
         <v>2</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D16*E16</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -768,10 +783,11 @@
         <v>3</v>
       </c>
       <c r="F17" s="0" t="n">
+        <f aca="false">D17*E17</f>
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -782,7 +798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -799,10 +815,11 @@
         <v>4</v>
       </c>
       <c r="F19" s="0" t="n">
+        <f aca="false">D19*E19</f>
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -819,10 +836,11 @@
         <v>5</v>
       </c>
       <c r="F20" s="0" t="n">
+        <f aca="false">D20*E20</f>
         <v>15</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -839,10 +857,11 @@
         <v>2</v>
       </c>
       <c r="F21" s="0" t="n">
+        <f aca="false">D21*E21</f>
         <v>4</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -859,10 +878,11 @@
         <v>4</v>
       </c>
       <c r="F22" s="0" t="n">
+        <f aca="false">D22*E22</f>
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>2</v>
       </c>
@@ -873,7 +893,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -884,7 +904,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -901,10 +921,11 @@
         <v>5</v>
       </c>
       <c r="F25" s="0" t="n">
+        <f aca="false">D25*E25</f>
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -921,10 +942,11 @@
         <v>0.5</v>
       </c>
       <c r="F26" s="0" t="n">
+        <f aca="false">D26*E26</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -941,10 +963,11 @@
         <v>0.5</v>
       </c>
       <c r="F27" s="0" t="n">
+        <f aca="false">D27*E27</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -961,10 +984,11 @@
         <v>1</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D28*E28</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -981,10 +1005,11 @@
         <v>0.5</v>
       </c>
       <c r="F29" s="0" t="n">
+        <f aca="false">D29*E29</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -1001,10 +1026,11 @@
         <v>0.5</v>
       </c>
       <c r="F30" s="0" t="n">
+        <f aca="false">D30*E30</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
@@ -1021,10 +1047,11 @@
         <v>2</v>
       </c>
       <c r="F31" s="0" t="n">
+        <f aca="false">D31*E31</f>
         <v>4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -1041,10 +1068,11 @@
         <v>0.5</v>
       </c>
       <c r="F32" s="0" t="n">
+        <f aca="false">D32*E32</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
@@ -1061,10 +1089,11 @@
         <v>0.5</v>
       </c>
       <c r="F33" s="0" t="n">
+        <f aca="false">D33*E33</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>3</v>
       </c>
@@ -1075,7 +1104,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>101</v>
       </c>
@@ -1092,10 +1121,11 @@
         <v>1</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">D35*E35</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>104</v>
       </c>
@@ -1112,10 +1142,14 @@
         <v>1</v>
       </c>
       <c r="F36" s="0" t="n">
+        <f aca="false">D36*E36</f>
         <v>3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="0" t="s">
+        <v>107</v>
+      </c>
       <c r="E37" s="0" t="n">
         <f aca="false">SUM(E4:E36)</f>
         <v>84</v>

</xml_diff>

<commit_message>
WBS uppdaterad, Aktivitetslista och Riskanalys skapade och färdigställda
</commit_message>
<xml_diff>
--- a/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
+++ b/Bolaget/Förstudie/WBS/WBS v.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beije\Documents\Projektkurs DVA227\Bolaget\Förstudie\WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C383E-67EB-46B2-80C7-314518F8D840}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9F93F5-5CF6-46E0-B233-8C3B422DD8D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{27FDFA86-4B27-4D7C-8CA5-C51076384BD6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -331,6 +331,24 @@
   </si>
   <si>
     <t>Total tid (Tidsåtgång x resurs)</t>
+  </si>
+  <si>
+    <t>Beroenden</t>
+  </si>
+  <si>
+    <t>1.1.5, 3.1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1.3.1, 1.3.2, 1.3.3</t>
+  </si>
+  <si>
+    <t>1.1.1, 1.1.2, 1.1.3, 1.1.4</t>
+  </si>
+  <si>
+    <t>1-</t>
   </si>
 </sst>
 </file>
@@ -366,10 +384,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37737CB-10EF-4991-AA29-BCEE5EE5F7F0}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,9 +719,11 @@
     <col min="3" max="3" width="88" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,8 +742,11 @@
       <c r="F1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -731,7 +757,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -742,7 +768,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,8 +787,11 @@
       <c r="F4">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -781,8 +810,11 @@
       <c r="F5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -801,8 +833,11 @@
       <c r="F6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -821,8 +856,11 @@
       <c r="F7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -841,8 +879,11 @@
       <c r="F8">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -861,8 +902,11 @@
       <c r="F9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1.2</v>
       </c>
@@ -873,7 +917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -892,8 +936,11 @@
       <c r="F11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -903,17 +950,8 @@
       <c r="C12" t="s">
         <v>77</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -932,8 +970,11 @@
       <c r="F13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -952,8 +993,11 @@
       <c r="F14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -972,8 +1016,11 @@
       <c r="F15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -992,8 +1039,11 @@
       <c r="F16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1012,8 +1062,11 @@
       <c r="F17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1.3</v>
       </c>
@@ -1024,7 +1077,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1043,8 +1096,11 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1063,8 +1119,11 @@
       <c r="F20">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1083,8 +1142,11 @@
       <c r="F21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1.4</v>
       </c>
@@ -1095,7 +1157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1114,8 +1176,11 @@
       <c r="F23">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1126,7 +1191,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2.1</v>
       </c>
@@ -1137,7 +1202,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1156,8 +1221,11 @@
       <c r="F26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1176,8 +1244,11 @@
       <c r="F27">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
@@ -1196,8 +1267,11 @@
       <c r="F28">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1216,8 +1290,11 @@
       <c r="F29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
@@ -1236,8 +1313,11 @@
       <c r="F30">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -1256,8 +1336,11 @@
       <c r="F31">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1276,8 +1359,11 @@
       <c r="F32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
@@ -1296,8 +1382,11 @@
       <c r="F33">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1317,7 +1406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -1327,8 +1416,11 @@
       <c r="C35" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>3.1</v>
       </c>
@@ -1347,8 +1439,11 @@
       <c r="F36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3.2</v>
       </c>
@@ -1367,15 +1462,18 @@
       <c r="F37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E38">
         <f>SUM(E4:E37)</f>
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F38">
         <f>SUM(F4:F37)</f>
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>